<commit_message>
Added version 1.04  of PCB
</commit_message>
<xml_diff>
--- a/Kicad/ElectronULA - MAX 10 Board V1.03/BOM.xlsx
+++ b/Kicad/ElectronULA - MAX 10 Board V1.03/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kiCAD\Projects\ElectronULA - MAX 10 Board - V1.03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ElectronULA\Kicad\ElectronULA - MAX 10 Board V1.03\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ElectronULA" localSheetId="0">Sheet1!$A$15:$I$33</definedName>
+    <definedName name="ElectronULA" localSheetId="0">Sheet1!$A$14:$I$32</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="90">
   <si>
     <t>Id</t>
   </si>
@@ -282,28 +282,6 @@
     <t>Excellent drag soldering guide here "https://www.youtube.com/watch?v=nyele3CIs-U"</t>
   </si>
   <si>
-    <t>https://www.ebay.co.uk/i/292483310138?chn=ps&amp;norover=1&amp;mkevt=1&amp;mkrid=710-134428-41853-0&amp;mkcid=2&amp;itemid=292483310138&amp;targetid=908661474856&amp;device=c&amp;mktype=pla&amp;googleloc=9046613&amp;poi=&amp;campaignid=10195651586&amp;mkgroupid=107296210212&amp;rlsatarget=pla-908661474856&amp;abcId=1145987&amp;merchantid=7398364&amp;gclid=EAIaIQobChMI6ru5t-WQ6gIVzoKyCh1oBwxIEAQYCiABEgImJvD_BwE</t>
-  </si>
-  <si>
-    <t>Note: This board can only be fitted to a PGA68 socket on the Electron board. This requires that the original ULA and socket are removed and replaced with a turned pin PGA68 socket</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Fit the ULA socket pins last (15). I would recommend "tinning" the pins which go into the ULA socket before fitting to the board otherwise they are a loose fit in the socket. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Check on your socket before doing this though just in case</t>
-    </r>
-  </si>
-  <si>
     <t>3. I recommend using a gel like flux for the SMD chips. Run plenty along each row of pads and then align the chip correctly, the gel helps keep the chip in place. Tag each corner by soldering one or two pins and then drag solder the rest. See guide below</t>
   </si>
   <si>
@@ -323,6 +301,24 @@
   </si>
   <si>
     <t>4.7K Resistor</t>
+  </si>
+  <si>
+    <t>Turned pin socket headers to make ULA socket for Electron circuit board</t>
+  </si>
+  <si>
+    <t>ULA Socket for Electron circuit board</t>
+  </si>
+  <si>
+    <t>Pack of 5 x 40 pin</t>
+  </si>
+  <si>
+    <t>https://hobbycomponents.com/connectors/392-01-254mm-40way-sil-turned-pin-m-f-headers-pack-of-5</t>
+  </si>
+  <si>
+    <t>1. Fit the ULA socket pins last (16)</t>
+  </si>
+  <si>
+    <t>Note: This board can only be fitted to a PGA68 socket on the Electron board. This requires that the original ULA and socket are removed and replaced with a turned pin PGA68 socket. This can be made from turned pin headers which is included in the BOM below</t>
   </si>
 </sst>
 </file>
@@ -454,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -494,6 +490,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -783,9 +785,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -799,7 +803,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -815,25 +819,25 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>77</v>
-      </c>
+      <c r="A5" s="1"/>
       <c r="B5" s="16"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="16"/>
+      <c r="A6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="1"/>
+      <c r="A7" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
@@ -843,464 +847,469 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>1</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="17">
+        <v>4</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>2</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
-        <v>1</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="17">
-        <v>4</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" s="17"/>
+      <c r="B16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>2</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="2">
-        <v>2</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D18" s="3">
+        <v>19</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>5</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="3">
         <v>1</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>4</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="3">
-        <v>19</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="12"/>
+        <v>14</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>44</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" s="11"/>
+        <v>67</v>
+      </c>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D22" s="3">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>67</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F22" s="3"/>
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D23" s="3">
+        <v>1</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>10</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="12"/>
-    </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
-        <v>9</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D26" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G26" s="11" t="s">
-        <v>63</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F26" s="3"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D27" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="12"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D28" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="12"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D29" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>65</v>
+        <v>35</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="D30" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D31" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="G31" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>18</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>40</v>
+        <v>74</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="15"/>
+    </row>
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>19</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>84</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="15"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="15"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>87</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G17" r:id="rId1"/>
-    <hyperlink ref="G20" r:id="rId2"/>
-    <hyperlink ref="G30" r:id="rId3"/>
-    <hyperlink ref="G32" r:id="rId4"/>
-    <hyperlink ref="G26" r:id="rId5" display="https://www.digikey.co.uk/product-detail/en/diodes-incorporated/AP2114H-3.3TRG1/AP2114H-3.3TRG1DICT-ND/4505142?utm_adgroup=PMIC%20-%20Voltage%20Regulators%20-%20Linear&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Google%20Shopping_Integrated%20Circuits%20%28ICs%29&amp;utm_term=&amp;productid=4505142&amp;gclid=EAIaIQobChMIkoq-teuO6gIVC4myCh0O7wooEAQYASABEgJpyfD_BwE"/>
-    <hyperlink ref="G29" r:id="rId6"/>
-    <hyperlink ref="G31" r:id="rId7"/>
-    <hyperlink ref="G18" r:id="rId8"/>
-    <hyperlink ref="A5" r:id="rId9" display="https://www.ebay.co.uk/i/292483310138?chn=ps&amp;norover=1&amp;mkevt=1&amp;mkrid=710-134428-41853-0&amp;mkcid=2&amp;itemid=292483310138&amp;targetid=908661474856&amp;device=c&amp;mktype=pla&amp;googleloc=9046613&amp;poi=&amp;campaignid=10195651586&amp;mkgroupid=107296210212&amp;rlsatarget=pla-908661474856&amp;abcId=1145987&amp;merchantid=7398364&amp;gclid=EAIaIQobChMI6ru5t-WQ6gIVzoKyCh1oBwxIEAQYCiABEgImJvD_BwE"/>
+    <hyperlink ref="G16" r:id="rId1"/>
+    <hyperlink ref="G19" r:id="rId2"/>
+    <hyperlink ref="G29" r:id="rId3"/>
+    <hyperlink ref="G31" r:id="rId4"/>
+    <hyperlink ref="G25" r:id="rId5" display="https://www.digikey.co.uk/product-detail/en/diodes-incorporated/AP2114H-3.3TRG1/AP2114H-3.3TRG1DICT-ND/4505142?utm_adgroup=PMIC%20-%20Voltage%20Regulators%20-%20Linear&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Google%20Shopping_Integrated%20Circuits%20%28ICs%29&amp;utm_term=&amp;productid=4505142&amp;gclid=EAIaIQobChMIkoq-teuO6gIVC4myCh0O7wooEAQYASABEgJpyfD_BwE"/>
+    <hyperlink ref="G28" r:id="rId6"/>
+    <hyperlink ref="G30" r:id="rId7"/>
+    <hyperlink ref="G17" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="42" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId10"/>
+  <pageSetup paperSize="9" scale="42" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>